<commit_message>
Fix exports for activities
</commit_message>
<xml_diff>
--- a/app/views/Exports/bySelectedActivity.xlsx
+++ b/app/views/Exports/bySelectedActivity.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FE2D2E-F7E6-524E-A5DD-1F216CEA2133}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AE7D17-C25B-5B4E-9309-86A33C5D1574}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="3940" windowWidth="19200" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="2700" windowWidth="26060" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>&lt;/jx:forEach&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -37,9 +37,6 @@
     <t>${assignment.studentChoices.student.name}</t>
   </si>
   <si>
-    <t>${assignment.schoolEventGroupActivity.schoolEventGroup.name}</t>
-  </si>
-  <si>
     <t>Classroom</t>
   </si>
   <si>
@@ -49,30 +46,44 @@
     <t>${proposal.name}</t>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>Activity</t>
   </si>
   <si>
     <t>${activity.name}</t>
   </si>
   <si>
-    <t>&lt;jx:forEach items="${assignments}" var="assignment"&gt;</t>
-  </si>
-  <si>
     <t>${assignment.studentChoices.student.classroom.name}</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${group.items}" var="assignment"&gt;</t>
+  </si>
+  <si>
+    <t>Abs Fri</t>
+  </si>
+  <si>
+    <t>Abs Sat</t>
+  </si>
+  <si>
+    <t>${assignment.studentChoices.absentSaturday?'x:''}</t>
+  </si>
+  <si>
+    <t>${assignment.studentChoices.absentFriday?'x':''}</t>
+  </si>
+  <si>
+    <t>${group.item.schoolEventGroupActivity.schoolEventGroup.name}</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${assignments}"  groupBy="schoolEventGroupActivity.schoolEventGroup.name" groupOrder="asc"&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="\$#,##0.00;\-\$#,##0.00"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +113,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -159,7 +178,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -184,20 +203,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,99 +553,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="23" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="18">
-      <c r="B2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="2:5" ht="18">
-      <c r="B3" s="9" t="s">
+    <row r="2" spans="2:6" ht="18">
+      <c r="B2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="2:6" ht="18">
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="2:5">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="2:6">
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="2:5">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="2"/>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:6">
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="5"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="5" t="s">
+      <c r="D9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="7" t="s">
+      <c r="F9" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="1" t="s">
+      <c r="D11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>